<commit_message>
add re-assign network code feature
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\catalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518A82DD-0361-4502-9840-F8DE811CC2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C91D62-EF27-4CE4-9FBA-EBA35B3EEE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="43">
   <si>
     <t>2024</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>s_arr_sec</t>
+  </si>
+  <si>
+    <t>KJ</t>
+  </si>
+  <si>
+    <t>network_code</t>
   </si>
 </sst>
 </file>
@@ -489,56 +495,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="8" max="8" width="18.3984375" customWidth="1"/>
-    <col min="12" max="12" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" customWidth="1"/>
+    <col min="13" max="13" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -546,1980 +556,2137 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="U1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>36.65205383</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
       <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>37.180698390000003</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1001</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>36.706321719999998</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>4</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>37.257804870000001</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1001</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>36.727073670000003</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
       <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>37.32366562</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>36.8090744</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
       <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
         <v>7</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>4</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>37.316196439999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1001</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>36.99797058</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
       <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
         <v>7</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>37.776321410000001</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1001</v>
       </c>
       <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>37.322792049999997</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
       <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
         <v>4</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>38.323970789999997</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1002</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>29.055486680000001</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
       <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
         <v>10</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>29.58934021</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1002</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>29.148645399999999</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>5</v>
       </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
       <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
         <v>10</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>29.71233368</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1002</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>29.15431976</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>5</v>
       </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
       <c r="K10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" t="s">
         <v>10</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>29.65493584</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1002</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>29.16581154</v>
       </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
       <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
         <v>7</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>10</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>29.672574999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1002</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>29.265352249999999</v>
       </c>
-      <c r="I12" t="s">
-        <v>8</v>
-      </c>
       <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
         <v>7</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>29.906728739999998</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1002</v>
       </c>
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>29.388738629999999</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>5</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>7</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>30.155675890000001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1002</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
         <v>2</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>9</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>10</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>29.450801850000001</v>
       </c>
-      <c r="I14" t="s">
-        <v>8</v>
-      </c>
       <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" t="s">
         <v>7</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>10</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>30.22833443</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1002</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>29.509855269999999</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>5</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>7</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>10</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>30.29590988</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1002</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>2</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>10</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>29.58403015</v>
       </c>
-      <c r="I16" t="s">
-        <v>8</v>
-      </c>
       <c r="J16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" t="s">
         <v>10</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>30.480550770000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1002</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>2</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>9</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>10</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>29.661956790000001</v>
       </c>
-      <c r="I17" t="s">
-        <v>8</v>
-      </c>
       <c r="J17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" t="s">
         <v>10</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>30.54605484</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1002</v>
       </c>
       <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>29.664175029999999</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>5</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>7</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>10</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>30.534849170000001</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1003</v>
       </c>
       <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>7.6824560200000001</v>
       </c>
-      <c r="I19" t="s">
-        <v>8</v>
-      </c>
       <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
         <v>7</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>13</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>8.3003301599999997</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1003</v>
       </c>
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>7.7048234899999999</v>
       </c>
-      <c r="I20" t="s">
-        <v>8</v>
-      </c>
       <c r="J20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" t="s">
         <v>13</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>8.3164444</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1003</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
         <v>13</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>7.7606349000000003</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>5</v>
       </c>
-      <c r="J21" t="s">
-        <v>6</v>
-      </c>
       <c r="K21" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" t="s">
         <v>13</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>8.3707542400000001</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1003</v>
       </c>
       <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="C22" t="s">
-        <v>0</v>
-      </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
         <v>13</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>7.78265429</v>
       </c>
-      <c r="I22" t="s">
-        <v>8</v>
-      </c>
       <c r="J22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" t="s">
         <v>13</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>8.5112981800000007</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>1003</v>
       </c>
       <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
         <v>13</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>7.7888274199999996</v>
       </c>
-      <c r="I23" t="s">
-        <v>8</v>
-      </c>
       <c r="J23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K23" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" t="s">
         <v>13</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>8.4920940399999996</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1003</v>
       </c>
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
         <v>13</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>7.8545846900000003</v>
       </c>
-      <c r="I24" t="s">
-        <v>8</v>
-      </c>
       <c r="J24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" t="s">
         <v>13</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>8.6193723700000007</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>1003</v>
       </c>
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>7.9642167099999996</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>5</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>7</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>13</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>8.7773723599999993</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1003</v>
       </c>
       <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
         <v>13</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>8.0202302900000007</v>
       </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
       <c r="J26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
         <v>7</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>13</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>8.85911179</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>1003</v>
       </c>
       <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
         <v>20</v>
       </c>
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
         <v>13</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>8.19187069</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>5</v>
       </c>
-      <c r="J27" t="s">
-        <v>6</v>
-      </c>
       <c r="K27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" t="s">
         <v>13</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>9.1689376800000009</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1003</v>
       </c>
       <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
         <v>13</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>8.2596292499999997</v>
       </c>
-      <c r="I28" t="s">
-        <v>8</v>
-      </c>
       <c r="J28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
         <v>13</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>9.2613372799999993</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1003</v>
       </c>
       <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
-        <v>0</v>
-      </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
         <v>13</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>8.2825441400000006</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>5</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>7</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>13</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>9.3555107100000008</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1003</v>
       </c>
       <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
         <v>13</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>8.3237772000000003</v>
       </c>
-      <c r="I30" t="s">
-        <v>8</v>
-      </c>
       <c r="J30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" t="s">
         <v>13</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>9.4120407099999994</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>1003</v>
       </c>
       <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="C31" t="s">
-        <v>0</v>
-      </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
         <v>13</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>8.4314098400000006</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>5</v>
       </c>
-      <c r="J31" t="s">
-        <v>6</v>
-      </c>
       <c r="K31" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" t="s">
         <v>13</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>9.5589571000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>1004</v>
       </c>
       <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
         <v>14</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>5.0248794600000002</v>
       </c>
-      <c r="I32" t="s">
-        <v>8</v>
-      </c>
       <c r="J32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" t="s">
         <v>14</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>5.7035388899999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>1004</v>
       </c>
       <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
-        <v>0</v>
-      </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
         <v>14</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>5.0281658199999999</v>
       </c>
-      <c r="I33" t="s">
-        <v>8</v>
-      </c>
       <c r="J33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" t="s">
         <v>7</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>14</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>5.7039380099999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>1004</v>
       </c>
       <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
         <v>18</v>
       </c>
-      <c r="C34" t="s">
-        <v>0</v>
-      </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
         <v>14</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>5.07122326</v>
       </c>
-      <c r="I34" t="s">
-        <v>8</v>
-      </c>
       <c r="J34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K34" t="s">
+        <v>6</v>
+      </c>
+      <c r="L34" t="s">
         <v>14</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>5.8260760300000003</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>1004</v>
       </c>
       <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
         <v>17</v>
       </c>
-      <c r="C35" t="s">
-        <v>0</v>
-      </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
         <v>14</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>5.0961909299999997</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>5</v>
       </c>
-      <c r="J35" t="s">
-        <v>6</v>
-      </c>
       <c r="K35" t="s">
+        <v>6</v>
+      </c>
+      <c r="L35" t="s">
         <v>14</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>5.85814667</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>1004</v>
       </c>
       <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
         <v>14</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>5.0971674900000004</v>
       </c>
-      <c r="I36" t="s">
-        <v>8</v>
-      </c>
       <c r="J36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" t="s">
         <v>14</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>5.8213386500000004</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>1004</v>
       </c>
       <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
         <v>14</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>5.1650395400000004</v>
       </c>
-      <c r="I37" t="s">
-        <v>8</v>
-      </c>
       <c r="J37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" t="s">
         <v>7</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>14</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>5.9157786400000001</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>1004</v>
       </c>
       <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
         <v>23</v>
       </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s">
         <v>14</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>5.3555522</v>
       </c>
-      <c r="I38" t="s">
-        <v>8</v>
-      </c>
       <c r="J38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K38" t="s">
+        <v>6</v>
+      </c>
+      <c r="L38" t="s">
         <v>14</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>6.2094521499999997</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>1004</v>
       </c>
       <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
         <v>24</v>
       </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
         <v>14</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>5.35674429</v>
       </c>
-      <c r="I39" t="s">
-        <v>8</v>
-      </c>
       <c r="J39" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" t="s">
         <v>7</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>14</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>6.21624088</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>1004</v>
       </c>
       <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
         <v>14</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>5.39427185</v>
       </c>
-      <c r="I40" t="s">
-        <v>8</v>
-      </c>
       <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" t="s">
         <v>7</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>14</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>6.3793225299999996</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>1004</v>
       </c>
       <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
         <v>21</v>
       </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
         <v>14</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>5.41018534</v>
       </c>
-      <c r="I41" t="s">
-        <v>8</v>
-      </c>
       <c r="J41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" t="s">
         <v>7</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>14</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>6.3798952099999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>1004</v>
       </c>
       <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
         <v>25</v>
       </c>
-      <c r="C42" t="s">
-        <v>0</v>
-      </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s">
         <v>14</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>5.5751848199999996</v>
       </c>
-      <c r="I42" t="s">
-        <v>8</v>
-      </c>
       <c r="J42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K42" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" t="s">
         <v>14</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>6.6634359400000003</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>1004</v>
       </c>
       <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
         <v>26</v>
       </c>
-      <c r="C43" t="s">
-        <v>0</v>
-      </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G43" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s">
         <v>14</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>5.6731581699999998</v>
       </c>
-      <c r="I43" t="s">
-        <v>8</v>
-      </c>
       <c r="J43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K43" t="s">
+        <v>6</v>
+      </c>
+      <c r="L43" t="s">
         <v>14</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>6.8367204700000004</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>1004</v>
       </c>
       <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
         <v>28</v>
       </c>
-      <c r="C44" t="s">
-        <v>0</v>
-      </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
         <v>14</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>5.7683205600000003</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>5</v>
       </c>
-      <c r="J44" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" t="s">
         <v>14</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>7.0342869800000001</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>1005</v>
       </c>
       <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
         <v>16</v>
       </c>
-      <c r="C45" t="s">
-        <v>0</v>
-      </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
         <v>15</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>13.1623354</v>
       </c>
-      <c r="I45" t="s">
-        <v>8</v>
-      </c>
       <c r="J45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K45" t="s">
+        <v>6</v>
+      </c>
+      <c r="L45" t="s">
         <v>15</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>13.82183933</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>1005</v>
       </c>
       <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" t="s">
         <v>18</v>
       </c>
-      <c r="C46" t="s">
-        <v>0</v>
-      </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
         <v>15</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>13.198514940000001</v>
       </c>
-      <c r="I46" t="s">
-        <v>8</v>
-      </c>
       <c r="J46" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" t="s">
         <v>7</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>15</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>13.867020610000001</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>1005</v>
       </c>
       <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s">
         <v>19</v>
       </c>
-      <c r="C47" t="s">
-        <v>0</v>
-      </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
         <v>15</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>13.216300009999999</v>
       </c>
-      <c r="I47" t="s">
-        <v>8</v>
-      </c>
       <c r="J47" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" t="s">
         <v>7</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>15</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>13.85861588</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>1005</v>
       </c>
       <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
         <v>17</v>
       </c>
-      <c r="C48" t="s">
-        <v>0</v>
-      </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
         <v>15</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>13.22078323</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>5</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>7</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>15</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>13.81419563</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>1005</v>
       </c>
       <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
         <v>27</v>
       </c>
-      <c r="C49" t="s">
-        <v>0</v>
-      </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
         <v>15</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>13.330042840000001</v>
       </c>
-      <c r="I49" t="s">
-        <v>8</v>
-      </c>
       <c r="J49" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" t="s">
         <v>7</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>15</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>14.029447559999999</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>1005</v>
       </c>
       <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
         <v>23</v>
       </c>
-      <c r="C50" t="s">
-        <v>0</v>
-      </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
         <v>15</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>13.47736359</v>
       </c>
-      <c r="I50" t="s">
-        <v>8</v>
-      </c>
       <c r="J50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K50" t="s">
+        <v>6</v>
+      </c>
+      <c r="L50" t="s">
         <v>15</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>14.32044411</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>1005</v>
       </c>
       <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
         <v>21</v>
       </c>
-      <c r="C51" t="s">
-        <v>0</v>
-      </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
         <v>15</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>13.60863209</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>5</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>7</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>15</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>14.524893759999999</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>1005</v>
       </c>
       <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
         <v>25</v>
       </c>
-      <c r="C52" t="s">
-        <v>0</v>
-      </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s">
         <v>15</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>13.707206729999999</v>
       </c>
-      <c r="I52" t="s">
-        <v>8</v>
-      </c>
       <c r="J52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K52" t="s">
+        <v>6</v>
+      </c>
+      <c r="L52" t="s">
         <v>15</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>14.708970069999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>1005</v>
       </c>
       <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
         <v>28</v>
       </c>
-      <c r="C53" t="s">
-        <v>0</v>
-      </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
         <v>15</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>13.96752262</v>
       </c>
-      <c r="I53" t="s">
-        <v>8</v>
-      </c>
       <c r="J53" t="s">
+        <v>8</v>
+      </c>
+      <c r="K53" t="s">
         <v>7</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>15</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>15.19153786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove network re-assignment,not necessary
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD78C9D-A04C-42ED-98B5-13968CF03149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6012389C-884C-4C56-8500-65A4B86E5DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="41">
   <si>
     <t>2024</t>
   </si>
@@ -148,12 +148,6 @@
   </si>
   <si>
     <t>s_arr_sec</t>
-  </si>
-  <si>
-    <t>KJ</t>
-  </si>
-  <si>
-    <t>network_code</t>
   </si>
 </sst>
 </file>
@@ -495,60 +489,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.3984375" customWidth="1"/>
-    <col min="13" max="13" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -556,2137 +547,1980 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="H2">
         <v>36.65205383</v>
       </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
       <c r="J2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="L2">
         <v>37.180698390000003</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1001</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>36.706321719999998</v>
       </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" t="s">
         <v>4</v>
       </c>
-      <c r="M3">
+      <c r="L3">
         <v>37.257804870000001</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1001</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <v>36.727073670000003</v>
       </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
       <c r="J4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="M4">
+      <c r="L4">
         <v>37.32366562</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="H5">
         <v>36.8090744</v>
       </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
       <c r="J5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" t="s">
         <v>4</v>
       </c>
-      <c r="M5">
+      <c r="L5">
         <v>37.316196439999999</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1001</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>36.99797058</v>
       </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="L6">
         <v>37.776321410000001</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1001</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="H7">
         <v>37.322792049999997</v>
       </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
       <c r="J7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
         <v>4</v>
       </c>
-      <c r="M7">
+      <c r="L7">
         <v>38.323970789999997</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1002</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="I8">
+      <c r="H8">
         <v>29.055486680000001</v>
       </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
       <c r="J8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
         <v>10</v>
       </c>
-      <c r="M8">
+      <c r="L8">
         <v>29.58934021</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1002</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="I9">
+      <c r="H9">
         <v>29.148645399999999</v>
       </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
       <c r="J9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="L9">
         <v>29.71233368</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1002</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="I10">
+      <c r="H10">
         <v>29.15431976</v>
       </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
       <c r="J10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
         <v>10</v>
       </c>
-      <c r="M10">
+      <c r="L10">
         <v>29.65493584</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1002</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="H11">
         <v>29.16581154</v>
       </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" t="s">
         <v>10</v>
       </c>
-      <c r="M11">
+      <c r="L11">
         <v>29.672574999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1002</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="I12">
+      <c r="H12">
         <v>29.265352249999999</v>
       </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="M12">
+      <c r="L12">
         <v>29.906728739999998</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1002</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
         <v>10</v>
       </c>
-      <c r="I13">
+      <c r="H13">
         <v>29.388738629999999</v>
       </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
       <c r="J13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" t="s">
         <v>10</v>
       </c>
-      <c r="M13">
+      <c r="L13">
         <v>30.155675890000001</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1002</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
         <v>10</v>
       </c>
-      <c r="I14">
+      <c r="H14">
         <v>29.450801850000001</v>
       </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
       <c r="J14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" t="s">
         <v>10</v>
       </c>
-      <c r="M14">
+      <c r="L14">
         <v>30.22833443</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1002</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" t="s">
         <v>10</v>
       </c>
-      <c r="I15">
+      <c r="H15">
         <v>29.509855269999999</v>
       </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
       <c r="J15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" t="s">
         <v>10</v>
       </c>
-      <c r="M15">
+      <c r="L15">
         <v>30.29590988</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1002</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" t="s">
         <v>10</v>
       </c>
-      <c r="I16">
+      <c r="H16">
         <v>29.58403015</v>
       </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
       <c r="J16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" t="s">
         <v>10</v>
       </c>
-      <c r="M16">
+      <c r="L16">
         <v>30.480550770000001</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1002</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
         <v>10</v>
       </c>
-      <c r="I17">
+      <c r="H17">
         <v>29.661956790000001</v>
       </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
       <c r="J17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" t="s">
         <v>10</v>
       </c>
-      <c r="M17">
+      <c r="L17">
         <v>30.54605484</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1002</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="I18">
+      <c r="H18">
         <v>29.664175029999999</v>
       </c>
+      <c r="I18" t="s">
+        <v>5</v>
+      </c>
       <c r="J18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K18" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" t="s">
         <v>10</v>
       </c>
-      <c r="M18">
+      <c r="L18">
         <v>30.534849170000001</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1003</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="I19">
+      <c r="H19">
         <v>7.6824560200000001</v>
       </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
       <c r="J19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K19" t="s">
-        <v>7</v>
-      </c>
-      <c r="L19" t="s">
         <v>13</v>
       </c>
-      <c r="M19">
+      <c r="L19">
         <v>8.3003301599999997</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1003</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="I20">
+      <c r="H20">
         <v>7.7048234899999999</v>
       </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
       <c r="J20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K20" t="s">
-        <v>6</v>
-      </c>
-      <c r="L20" t="s">
         <v>13</v>
       </c>
-      <c r="M20">
+      <c r="L20">
         <v>8.3164444</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1003</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
         <v>13</v>
       </c>
-      <c r="I21">
+      <c r="H21">
         <v>7.7606349000000003</v>
       </c>
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
       <c r="J21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" t="s">
-        <v>6</v>
-      </c>
-      <c r="L21" t="s">
         <v>13</v>
       </c>
-      <c r="M21">
+      <c r="L21">
         <v>8.3707542400000001</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1003</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" t="s">
         <v>13</v>
       </c>
-      <c r="I22">
+      <c r="H22">
         <v>7.78265429</v>
       </c>
+      <c r="I22" t="s">
+        <v>8</v>
+      </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L22" t="s">
         <v>13</v>
       </c>
-      <c r="M22">
+      <c r="L22">
         <v>8.5112981800000007</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1003</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
         <v>13</v>
       </c>
-      <c r="I23">
+      <c r="H23">
         <v>7.7888274199999996</v>
       </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
       <c r="J23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" t="s">
         <v>13</v>
       </c>
-      <c r="M23">
+      <c r="L23">
         <v>8.4920940399999996</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1003</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" t="s">
         <v>13</v>
       </c>
-      <c r="I24">
+      <c r="H24">
         <v>7.8545846900000003</v>
       </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
       <c r="J24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K24" t="s">
-        <v>6</v>
-      </c>
-      <c r="L24" t="s">
         <v>13</v>
       </c>
-      <c r="M24">
+      <c r="L24">
         <v>8.6193723700000007</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1003</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="I25">
+      <c r="H25">
         <v>7.9642167099999996</v>
       </c>
+      <c r="I25" t="s">
+        <v>5</v>
+      </c>
       <c r="J25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L25" t="s">
         <v>13</v>
       </c>
-      <c r="M25">
+      <c r="L25">
         <v>8.7773723599999993</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1003</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" t="s">
         <v>13</v>
       </c>
-      <c r="I26">
+      <c r="H26">
         <v>8.0202302900000007</v>
       </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
       <c r="J26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>7</v>
-      </c>
-      <c r="L26" t="s">
         <v>13</v>
       </c>
-      <c r="M26">
+      <c r="L26">
         <v>8.85911179</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1003</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
         <v>13</v>
       </c>
-      <c r="I27">
+      <c r="H27">
         <v>8.19187069</v>
       </c>
+      <c r="I27" t="s">
+        <v>5</v>
+      </c>
       <c r="J27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K27" t="s">
-        <v>6</v>
-      </c>
-      <c r="L27" t="s">
         <v>13</v>
       </c>
-      <c r="M27">
+      <c r="L27">
         <v>9.1689376800000009</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1003</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
         <v>13</v>
       </c>
-      <c r="I28">
+      <c r="H28">
         <v>8.2596292499999997</v>
       </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
       <c r="J28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K28" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" t="s">
         <v>13</v>
       </c>
-      <c r="M28">
+      <c r="L28">
         <v>9.2613372799999993</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1003</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" t="s">
         <v>13</v>
       </c>
-      <c r="I29">
+      <c r="H29">
         <v>8.2825441400000006</v>
       </c>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
       <c r="J29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K29" t="s">
-        <v>7</v>
-      </c>
-      <c r="L29" t="s">
         <v>13</v>
       </c>
-      <c r="M29">
+      <c r="L29">
         <v>9.3555107100000008</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1003</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" t="s">
         <v>13</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <v>8.3237772000000003</v>
       </c>
+      <c r="I30" t="s">
+        <v>8</v>
+      </c>
       <c r="J30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K30" t="s">
-        <v>6</v>
-      </c>
-      <c r="L30" t="s">
         <v>13</v>
       </c>
-      <c r="M30">
+      <c r="L30">
         <v>9.4120407099999994</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1003</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" t="s">
         <v>13</v>
       </c>
-      <c r="I31">
+      <c r="H31">
         <v>8.4314098400000006</v>
       </c>
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
       <c r="J31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" t="s">
         <v>13</v>
       </c>
-      <c r="M31">
+      <c r="L31">
         <v>9.5589571000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1004</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
         <v>14</v>
       </c>
-      <c r="I32">
+      <c r="H32">
         <v>5.0248794600000002</v>
       </c>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
       <c r="J32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K32" t="s">
-        <v>6</v>
-      </c>
-      <c r="L32" t="s">
         <v>14</v>
       </c>
-      <c r="M32">
+      <c r="L32">
         <v>5.7035388899999999</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1004</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
         <v>14</v>
       </c>
-      <c r="I33">
+      <c r="H33">
         <v>5.0281658199999999</v>
       </c>
+      <c r="I33" t="s">
+        <v>8</v>
+      </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K33" t="s">
-        <v>7</v>
-      </c>
-      <c r="L33" t="s">
         <v>14</v>
       </c>
-      <c r="M33">
+      <c r="L33">
         <v>5.7039380099999999</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1004</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
         <v>14</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <v>5.07122326</v>
       </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
       <c r="J34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K34" t="s">
-        <v>6</v>
-      </c>
-      <c r="L34" t="s">
         <v>14</v>
       </c>
-      <c r="M34">
+      <c r="L34">
         <v>5.8260760300000003</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1004</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
         <v>14</v>
       </c>
-      <c r="I35">
+      <c r="H35">
         <v>5.0961909299999997</v>
       </c>
+      <c r="I35" t="s">
+        <v>5</v>
+      </c>
       <c r="J35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K35" t="s">
-        <v>6</v>
-      </c>
-      <c r="L35" t="s">
         <v>14</v>
       </c>
-      <c r="M35">
+      <c r="L35">
         <v>5.85814667</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1004</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" t="s">
         <v>14</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <v>5.0971674900000004</v>
       </c>
+      <c r="I36" t="s">
+        <v>8</v>
+      </c>
       <c r="J36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K36" t="s">
-        <v>6</v>
-      </c>
-      <c r="L36" t="s">
         <v>14</v>
       </c>
-      <c r="M36">
+      <c r="L36">
         <v>5.8213386500000004</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1004</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s">
         <v>14</v>
       </c>
-      <c r="I37">
+      <c r="H37">
         <v>5.1650395400000004</v>
       </c>
+      <c r="I37" t="s">
+        <v>8</v>
+      </c>
       <c r="J37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K37" t="s">
-        <v>7</v>
-      </c>
-      <c r="L37" t="s">
         <v>14</v>
       </c>
-      <c r="M37">
+      <c r="L37">
         <v>5.9157786400000001</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1004</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" t="s">
         <v>14</v>
       </c>
-      <c r="I38">
+      <c r="H38">
         <v>5.3555522</v>
       </c>
+      <c r="I38" t="s">
+        <v>8</v>
+      </c>
       <c r="J38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K38" t="s">
-        <v>6</v>
-      </c>
-      <c r="L38" t="s">
         <v>14</v>
       </c>
-      <c r="M38">
+      <c r="L38">
         <v>6.2094521499999997</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1004</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
         <v>14</v>
       </c>
-      <c r="I39">
+      <c r="H39">
         <v>5.35674429</v>
       </c>
+      <c r="I39" t="s">
+        <v>8</v>
+      </c>
       <c r="J39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K39" t="s">
-        <v>7</v>
-      </c>
-      <c r="L39" t="s">
         <v>14</v>
       </c>
-      <c r="M39">
+      <c r="L39">
         <v>6.21624088</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1004</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" t="s">
         <v>14</v>
       </c>
-      <c r="I40">
+      <c r="H40">
         <v>5.39427185</v>
       </c>
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
       <c r="J40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K40" t="s">
-        <v>7</v>
-      </c>
-      <c r="L40" t="s">
         <v>14</v>
       </c>
-      <c r="M40">
+      <c r="L40">
         <v>6.3793225299999996</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1004</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
         <v>14</v>
       </c>
-      <c r="I41">
+      <c r="H41">
         <v>5.41018534</v>
       </c>
+      <c r="I41" t="s">
+        <v>8</v>
+      </c>
       <c r="J41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K41" t="s">
-        <v>7</v>
-      </c>
-      <c r="L41" t="s">
         <v>14</v>
       </c>
-      <c r="M41">
+      <c r="L41">
         <v>6.3798952099999999</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1004</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
         <v>14</v>
       </c>
-      <c r="I42">
+      <c r="H42">
         <v>5.5751848199999996</v>
       </c>
+      <c r="I42" t="s">
+        <v>8</v>
+      </c>
       <c r="J42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L42" t="s">
         <v>14</v>
       </c>
-      <c r="M42">
+      <c r="L42">
         <v>6.6634359400000003</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1004</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" t="s">
         <v>14</v>
       </c>
-      <c r="I43">
+      <c r="H43">
         <v>5.6731581699999998</v>
       </c>
+      <c r="I43" t="s">
+        <v>8</v>
+      </c>
       <c r="J43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K43" t="s">
-        <v>6</v>
-      </c>
-      <c r="L43" t="s">
         <v>14</v>
       </c>
-      <c r="M43">
+      <c r="L43">
         <v>6.8367204700000004</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1004</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" t="s">
         <v>14</v>
       </c>
-      <c r="I44">
+      <c r="H44">
         <v>5.7683205600000003</v>
       </c>
+      <c r="I44" t="s">
+        <v>5</v>
+      </c>
       <c r="J44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K44" t="s">
-        <v>6</v>
-      </c>
-      <c r="L44" t="s">
         <v>14</v>
       </c>
-      <c r="M44">
+      <c r="L44">
         <v>7.0342869800000001</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1005</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="s">
         <v>15</v>
       </c>
-      <c r="I45">
+      <c r="H45">
         <v>13.1623354</v>
       </c>
+      <c r="I45" t="s">
+        <v>8</v>
+      </c>
       <c r="J45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K45" t="s">
-        <v>6</v>
-      </c>
-      <c r="L45" t="s">
         <v>15</v>
       </c>
-      <c r="M45">
+      <c r="L45">
         <v>13.82183933</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1005</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" t="s">
         <v>15</v>
       </c>
-      <c r="I46">
+      <c r="H46">
         <v>13.198514940000001</v>
       </c>
+      <c r="I46" t="s">
+        <v>8</v>
+      </c>
       <c r="J46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K46" t="s">
-        <v>7</v>
-      </c>
-      <c r="L46" t="s">
         <v>15</v>
       </c>
-      <c r="M46">
+      <c r="L46">
         <v>13.867020610000001</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1005</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" t="s">
         <v>15</v>
       </c>
-      <c r="I47">
+      <c r="H47">
         <v>13.216300009999999</v>
       </c>
+      <c r="I47" t="s">
+        <v>8</v>
+      </c>
       <c r="J47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K47" t="s">
-        <v>7</v>
-      </c>
-      <c r="L47" t="s">
         <v>15</v>
       </c>
-      <c r="M47">
+      <c r="L47">
         <v>13.85861588</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1005</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" t="s">
         <v>15</v>
       </c>
-      <c r="I48">
+      <c r="H48">
         <v>13.22078323</v>
       </c>
+      <c r="I48" t="s">
+        <v>5</v>
+      </c>
       <c r="J48" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K48" t="s">
-        <v>7</v>
-      </c>
-      <c r="L48" t="s">
         <v>15</v>
       </c>
-      <c r="M48">
+      <c r="L48">
         <v>13.81419563</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1005</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" t="s">
         <v>15</v>
       </c>
-      <c r="I49">
+      <c r="H49">
         <v>13.330042840000001</v>
       </c>
+      <c r="I49" t="s">
+        <v>8</v>
+      </c>
       <c r="J49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K49" t="s">
-        <v>7</v>
-      </c>
-      <c r="L49" t="s">
         <v>15</v>
       </c>
-      <c r="M49">
+      <c r="L49">
         <v>14.029447559999999</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1005</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" t="s">
         <v>15</v>
       </c>
-      <c r="I50">
+      <c r="H50">
         <v>13.47736359</v>
       </c>
+      <c r="I50" t="s">
+        <v>8</v>
+      </c>
       <c r="J50" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K50" t="s">
-        <v>6</v>
-      </c>
-      <c r="L50" t="s">
         <v>15</v>
       </c>
-      <c r="M50">
+      <c r="L50">
         <v>14.32044411</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1005</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" t="s">
         <v>15</v>
       </c>
-      <c r="I51">
+      <c r="H51">
         <v>13.60863209</v>
       </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
       <c r="J51" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K51" t="s">
-        <v>7</v>
-      </c>
-      <c r="L51" t="s">
         <v>15</v>
       </c>
-      <c r="M51">
+      <c r="L51">
         <v>14.524893759999999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1005</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" t="s">
         <v>15</v>
       </c>
-      <c r="I52">
+      <c r="H52">
         <v>13.707206729999999</v>
       </c>
+      <c r="I52" t="s">
+        <v>8</v>
+      </c>
       <c r="J52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K52" t="s">
-        <v>6</v>
-      </c>
-      <c r="L52" t="s">
         <v>15</v>
       </c>
-      <c r="M52">
+      <c r="L52">
         <v>14.708970069999999</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1005</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" t="s">
         <v>15</v>
       </c>
-      <c r="I53">
+      <c r="H53">
         <v>13.96752262</v>
       </c>
+      <c r="I53" t="s">
+        <v>8</v>
+      </c>
       <c r="J53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K53" t="s">
-        <v>7</v>
-      </c>
-      <c r="L53" t="s">
         <v>15</v>
       </c>
-      <c r="M53">
+      <c r="L53">
         <v>15.19153786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add coda time to catalog, improve the require and output dataframe structur
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
+++ b/tests/sample_tests_data/data/catalog/picking_catalog.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\lqt-moment-magnitude\tests\sample_tests_data\data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF5B4B-E597-4D8A-8C53-121221B76C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EEF5BB-0515-402A-8B94-6C3855511054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="45">
   <si>
     <t>2024</t>
   </si>
@@ -129,9 +129,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>hour</t>
-  </si>
-  <si>
     <t>minute_p</t>
   </si>
   <si>
@@ -148,6 +145,21 @@
   </si>
   <si>
     <t>s_arr_sec</t>
+  </si>
+  <si>
+    <t>hour_p</t>
+  </si>
+  <si>
+    <t>hour_s</t>
+  </si>
+  <si>
+    <t>hour_coda</t>
+  </si>
+  <si>
+    <t>minute_coda</t>
+  </si>
+  <si>
+    <t>sec_coda</t>
   </si>
 </sst>
 </file>
@@ -492,14 +504,17 @@
   <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -519,30 +534,38 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -580,10 +603,23 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>37.180698390000003</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <f>M2+7</f>
+        <v>44.180698390000003</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -618,10 +654,23 @@
         <v>7</v>
       </c>
       <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>37.257804870000001</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P53" si="0">M3+7</f>
+        <v>44.257804870000001</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -656,10 +705,23 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>37.32366562</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>44.32366562</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -694,10 +756,23 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
         <v>4</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>37.316196439999999</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>44.316196439999999</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -732,10 +807,23 @@
         <v>7</v>
       </c>
       <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>37.776321410000001</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>44.776321410000001</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -770,10 +858,23 @@
         <v>6</v>
       </c>
       <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
         <v>4</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>38.323970789999997</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>45.323970789999997</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -808,10 +909,23 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
         <v>10</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>29.58934021</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>36.589340210000003</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -846,10 +960,23 @@
         <v>6</v>
       </c>
       <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
         <v>10</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>29.71233368</v>
+      </c>
+      <c r="N9" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>36.71233368</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -884,10 +1011,23 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
         <v>10</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>29.65493584</v>
+      </c>
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>36.65493584</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -922,10 +1062,23 @@
         <v>7</v>
       </c>
       <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
         <v>10</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>29.672574999999998</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>36.672574999999995</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -960,10 +1113,23 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>29.906728739999998</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>36.906728739999998</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -998,10 +1164,23 @@
         <v>7</v>
       </c>
       <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" t="s">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>30.155675890000001</v>
+      </c>
+      <c r="N13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>37.155675889999998</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1036,10 +1215,23 @@
         <v>7</v>
       </c>
       <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
         <v>10</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>30.22833443</v>
+      </c>
+      <c r="N14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>37.228334430000004</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1074,10 +1266,23 @@
         <v>7</v>
       </c>
       <c r="K15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" t="s">
         <v>10</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>30.29590988</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>37.295909879999996</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1112,13 +1317,26 @@
         <v>6</v>
       </c>
       <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" t="s">
         <v>10</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>30.480550770000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>37.480550770000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1002</v>
       </c>
@@ -1150,13 +1368,26 @@
         <v>6</v>
       </c>
       <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" t="s">
         <v>10</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>30.54605484</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>37.546054839999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1002</v>
       </c>
@@ -1188,13 +1419,26 @@
         <v>7</v>
       </c>
       <c r="K18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" t="s">
         <v>10</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>30.534849170000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>37.534849170000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1003</v>
       </c>
@@ -1226,13 +1470,26 @@
         <v>7</v>
       </c>
       <c r="K19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19">
+        <v>12</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19">
         <v>8.3003301599999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>15.30033016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1003</v>
       </c>
@@ -1264,13 +1521,26 @@
         <v>6</v>
       </c>
       <c r="K20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20">
+        <v>12</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20">
         <v>8.3164444</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>15.3164444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1003</v>
       </c>
@@ -1302,13 +1572,26 @@
         <v>6</v>
       </c>
       <c r="K21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21">
         <v>8.3707542400000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" t="s">
+        <v>13</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="0"/>
+        <v>15.37075424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1003</v>
       </c>
@@ -1340,13 +1623,26 @@
         <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22">
+        <v>12</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22">
         <v>8.5112981800000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>15.511298180000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1003</v>
       </c>
@@ -1378,13 +1674,26 @@
         <v>6</v>
       </c>
       <c r="K23" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23">
         <v>8.4920940399999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" t="s">
+        <v>13</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>15.49209404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1003</v>
       </c>
@@ -1416,13 +1725,26 @@
         <v>6</v>
       </c>
       <c r="K24" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24">
+        <v>12</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24">
         <v>8.6193723700000007</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>15.619372370000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1003</v>
       </c>
@@ -1454,13 +1776,26 @@
         <v>7</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25">
         <v>8.7773723599999993</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" t="s">
+        <v>13</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>15.777372359999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1003</v>
       </c>
@@ -1492,13 +1827,26 @@
         <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26">
+        <v>12</v>
+      </c>
+      <c r="L26" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26">
         <v>8.85911179</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" t="s">
+        <v>13</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>15.85911179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1003</v>
       </c>
@@ -1530,13 +1878,26 @@
         <v>6</v>
       </c>
       <c r="K27" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M27">
         <v>9.1689376800000009</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" t="s">
+        <v>13</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>16.168937679999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1003</v>
       </c>
@@ -1568,13 +1929,26 @@
         <v>6</v>
       </c>
       <c r="K28" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28">
+        <v>12</v>
+      </c>
+      <c r="L28" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28">
         <v>9.2613372799999993</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>16.261337279999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1003</v>
       </c>
@@ -1606,13 +1980,26 @@
         <v>7</v>
       </c>
       <c r="K29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L29">
+        <v>12</v>
+      </c>
+      <c r="L29" t="s">
+        <v>13</v>
+      </c>
+      <c r="M29">
         <v>9.3555107100000008</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" t="s">
+        <v>13</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>16.355510710000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1003</v>
       </c>
@@ -1644,13 +2031,26 @@
         <v>6</v>
       </c>
       <c r="K30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30">
+        <v>12</v>
+      </c>
+      <c r="L30" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30">
         <v>9.4120407099999994</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" t="s">
+        <v>13</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>16.412040709999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1003</v>
       </c>
@@ -1682,13 +2082,26 @@
         <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L31">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31">
         <v>9.5589571000000007</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" t="s">
+        <v>13</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>16.558957100000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1004</v>
       </c>
@@ -1720,13 +2133,26 @@
         <v>6</v>
       </c>
       <c r="K32" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32">
+        <v>12</v>
+      </c>
+      <c r="L32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32">
         <v>5.7035388899999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>12.703538890000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1004</v>
       </c>
@@ -1758,13 +2184,26 @@
         <v>7</v>
       </c>
       <c r="K33" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33">
+        <v>12</v>
+      </c>
+      <c r="L33" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33">
         <v>5.7039380099999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>12.70393801</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1004</v>
       </c>
@@ -1796,13 +2235,26 @@
         <v>6</v>
       </c>
       <c r="K34" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34">
+        <v>12</v>
+      </c>
+      <c r="L34" t="s">
+        <v>14</v>
+      </c>
+      <c r="M34">
         <v>5.8260760300000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>12.826076029999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1004</v>
       </c>
@@ -1834,13 +2286,26 @@
         <v>6</v>
       </c>
       <c r="K35" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35">
+        <v>12</v>
+      </c>
+      <c r="L35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M35">
         <v>5.85814667</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="s">
+        <v>14</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>12.85814667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1004</v>
       </c>
@@ -1872,13 +2337,26 @@
         <v>6</v>
       </c>
       <c r="K36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36">
+        <v>12</v>
+      </c>
+      <c r="L36" t="s">
+        <v>14</v>
+      </c>
+      <c r="M36">
         <v>5.8213386500000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
+        <v>14</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>12.821338650000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1004</v>
       </c>
@@ -1910,13 +2388,26 @@
         <v>7</v>
       </c>
       <c r="K37" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37">
+        <v>12</v>
+      </c>
+      <c r="L37" t="s">
+        <v>14</v>
+      </c>
+      <c r="M37">
         <v>5.9157786400000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" t="s">
+        <v>14</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>12.915778639999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1004</v>
       </c>
@@ -1948,13 +2439,26 @@
         <v>6</v>
       </c>
       <c r="K38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L38">
+        <v>12</v>
+      </c>
+      <c r="L38" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38">
         <v>6.2094521499999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" t="s">
+        <v>14</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>13.209452150000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1004</v>
       </c>
@@ -1986,13 +2490,26 @@
         <v>7</v>
       </c>
       <c r="K39" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39">
+        <v>12</v>
+      </c>
+      <c r="L39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39">
         <v>6.21624088</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" t="s">
+        <v>14</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>13.216240880000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1004</v>
       </c>
@@ -2024,13 +2541,26 @@
         <v>7</v>
       </c>
       <c r="K40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40">
+        <v>12</v>
+      </c>
+      <c r="L40" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40">
         <v>6.3793225299999996</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>12</v>
+      </c>
+      <c r="O40" t="s">
+        <v>14</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>13.37932253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1004</v>
       </c>
@@ -2062,13 +2592,26 @@
         <v>7</v>
       </c>
       <c r="K41" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41">
+        <v>12</v>
+      </c>
+      <c r="L41" t="s">
+        <v>14</v>
+      </c>
+      <c r="M41">
         <v>6.3798952099999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" t="s">
+        <v>14</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>13.379895210000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1004</v>
       </c>
@@ -2100,13 +2643,26 @@
         <v>6</v>
       </c>
       <c r="K42" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42">
+        <v>12</v>
+      </c>
+      <c r="L42" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42">
         <v>6.6634359400000003</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>12</v>
+      </c>
+      <c r="O42" t="s">
+        <v>14</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>13.663435939999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1004</v>
       </c>
@@ -2138,13 +2694,26 @@
         <v>6</v>
       </c>
       <c r="K43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43">
+        <v>12</v>
+      </c>
+      <c r="L43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M43">
         <v>6.8367204700000004</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>12</v>
+      </c>
+      <c r="O43" t="s">
+        <v>14</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>13.836720469999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1004</v>
       </c>
@@ -2176,13 +2745,26 @@
         <v>6</v>
       </c>
       <c r="K44" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44">
+        <v>12</v>
+      </c>
+      <c r="L44" t="s">
+        <v>14</v>
+      </c>
+      <c r="M44">
         <v>7.0342869800000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" t="s">
+        <v>14</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>14.034286980000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1005</v>
       </c>
@@ -2214,13 +2796,26 @@
         <v>6</v>
       </c>
       <c r="K45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" t="s">
         <v>15</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>13.82183933</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>12</v>
+      </c>
+      <c r="O45" t="s">
+        <v>15</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>20.82183933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1005</v>
       </c>
@@ -2252,13 +2847,26 @@
         <v>7</v>
       </c>
       <c r="K46" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" t="s">
         <v>15</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>13.867020610000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" t="s">
+        <v>15</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>20.867020610000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1005</v>
       </c>
@@ -2290,13 +2898,26 @@
         <v>7</v>
       </c>
       <c r="K47" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" t="s">
         <v>15</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>13.85861588</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" t="s">
+        <v>15</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="0"/>
+        <v>20.858615880000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1005</v>
       </c>
@@ -2328,13 +2949,26 @@
         <v>7</v>
       </c>
       <c r="K48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" t="s">
         <v>15</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>13.81419563</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" t="s">
+        <v>15</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="0"/>
+        <v>20.81419563</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1005</v>
       </c>
@@ -2366,13 +3000,26 @@
         <v>7</v>
       </c>
       <c r="K49" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" t="s">
         <v>15</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>14.029447559999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>12</v>
+      </c>
+      <c r="O49" t="s">
+        <v>15</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>21.029447560000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1005</v>
       </c>
@@ -2404,13 +3051,26 @@
         <v>6</v>
       </c>
       <c r="K50" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" t="s">
         <v>15</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>14.32044411</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O50" t="s">
+        <v>15</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>21.32044411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1005</v>
       </c>
@@ -2442,13 +3102,26 @@
         <v>7</v>
       </c>
       <c r="K51" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" t="s">
         <v>15</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>14.524893759999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" t="s">
+        <v>15</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="0"/>
+        <v>21.524893759999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1005</v>
       </c>
@@ -2480,13 +3153,26 @@
         <v>6</v>
       </c>
       <c r="K52" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" t="s">
         <v>15</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>14.708970069999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>12</v>
+      </c>
+      <c r="O52" t="s">
+        <v>15</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="0"/>
+        <v>21.708970069999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1005</v>
       </c>
@@ -2518,10 +3204,23 @@
         <v>7</v>
       </c>
       <c r="K53" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" t="s">
         <v>15</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>15.19153786</v>
+      </c>
+      <c r="N53" t="s">
+        <v>12</v>
+      </c>
+      <c r="O53" t="s">
+        <v>15</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="0"/>
+        <v>22.19153786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>